<commit_message>
Complete migration with tests working
</commit_message>
<xml_diff>
--- a/src/integration-test/resources/simpleImport.xlsx
+++ b/src/integration-test/resources/simpleImport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adjl/code/maurodatamapper-plugins/mdm-plugin-excel/src/integration-test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliverfreeman/code/mauro_data_mapper_plugins/mdm-plugin-excel/src/integration-test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2B99EB-A2CE-CF41-8346-DA456DB995E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5897E4B7-8005-0646-93FC-BF9FD9E18DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20280" activeTab="1" xr2:uid="{C2FC2BFD-8D7E-AA4E-A82C-4DBAFEC0EBFC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20280" activeTab="1" xr2:uid="{C2FC2BFD-8D7E-AA4E-A82C-4DBAFEC0EBFC}"/>
   </bookViews>
   <sheets>
     <sheet name="DataModels" sheetId="1" r:id="rId1"/>

</xml_diff>